<commit_message>
Ajout du backlog et repartition des taches de l'equipe
</commit_message>
<xml_diff>
--- a/backlogM2IL.xlsx
+++ b/backlogM2IL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>En tant que chef d'équipe j'ai besoin de valider la formation des salariés</t>
+  </si>
+  <si>
+    <t>GuillaumeNG</t>
+  </si>
+  <si>
+    <t>GeorgiaLR</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -436,11 +444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95236864"/>
-        <c:axId val="95238784"/>
+        <c:axId val="103110144"/>
+        <c:axId val="103112064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95236864"/>
+        <c:axId val="103110144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +457,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95238784"/>
+        <c:crossAx val="103112064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95238784"/>
+        <c:axId val="103112064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,21 +488,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95236864"/>
+        <c:crossAx val="103110144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -920,7 +926,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1035,9 @@
       <c r="F5" s="11">
         <v>8</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
@@ -1048,7 +1056,9 @@
       <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1067,7 +1077,9 @@
       <c r="F7" s="11">
         <v>13</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -1130,7 +1142,9 @@
       <c r="F10" s="11">
         <v>21</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>

</xml_diff>